<commit_message>
updated sustainable tourism goal
</commit_message>
<xml_diff>
--- a/prep_whi/TR/t_visitor_stats.xlsx
+++ b/prep_whi/TR/t_visitor_stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="10140" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,11 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -431,11 +432,11 @@
       <c r="D2" s="1">
         <v>9207726</v>
       </c>
-      <c r="E2" s="2">
-        <v>106.4</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1838.5</v>
+      <c r="E2" s="4">
+        <v>160.4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1839</v>
       </c>
       <c r="G2" s="2">
         <v>25227</v>
@@ -466,7 +467,7 @@
       <c r="E3">
         <v>172.2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>1896.2</v>
       </c>
       <c r="G3" s="3">
@@ -531,6 +532,23 @@
       </c>
       <c r="F6">
         <v>1498.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>2010</v>
+      </c>
+      <c r="C7">
+        <v>1378921</v>
+      </c>
+      <c r="D7">
+        <v>7284769</v>
+      </c>
+      <c r="E7">
+        <v>145.1</v>
+      </c>
+      <c r="F7">
+        <v>1345.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>